<commit_message>
machine learning book finished chapter 7
</commit_message>
<xml_diff>
--- a/ML001_20200901.xlsx
+++ b/ML001_20200901.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zephan\Qsync\Doc\ml001\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9888AC8-8688-4882-B228-961E4A2CAD15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="12450" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ml0201" sheetId="1" r:id="rId1"/>
     <sheet name="ml0301" sheetId="2" r:id="rId2"/>
     <sheet name="ml0601" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -48,361 +64,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;HK$&quot;* #,##0_);_(&quot;HK$&quot;* \(#,##0\);_(&quot;HK$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_(&quot;HK$&quot;* #,##0.00_);_(&quot;HK$&quot;* \(#,##0.00\);_(&quot;HK$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -410,251 +97,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -666,68 +111,24 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+  <cellStyles count="1">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -744,7 +145,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="marker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -774,9 +175,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
@@ -810,8 +208,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0667104111986002"/>
-                  <c:y val="0.300925925925926"/>
+                  <c:x val="-6.6710411198600203E-2"/>
+                  <c:y val="0.30092592592592599"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="#,##0.00_);[Red]\(#,##0.00\)" sourceLinked="0"/>
@@ -839,6 +237,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
+                  <a:endParaRPr lang="zh-CN"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -898,12 +297,17 @@
                   <c:v>16.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.1</c:v>
+                  <c:v>17.100000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0758-456B-8205-EDD71BDE80F9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -950,7 +354,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -995,6 +398,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="457693088"/>
@@ -1035,7 +439,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1080,6 +483,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="457692432"/>
@@ -1121,6 +525,7 @@
       <a:pPr>
         <a:defRPr lang="en-US"/>
       </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1132,7 +537,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -1149,7 +554,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="marker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1179,9 +584,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
@@ -1215,8 +617,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0667104111986002"/>
-                  <c:y val="0.300925925925926"/>
+                  <c:x val="-6.6710411198600203E-2"/>
+                  <c:y val="0.30092592592592599"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="#,##0.00_);[Red]\(#,##0.00\)" sourceLinked="0"/>
@@ -1244,6 +646,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
+                  <a:endParaRPr lang="zh-CN"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1309,6 +712,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E757-4B7D-8C2E-191135066524}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1355,7 +763,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1400,6 +807,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="457693088"/>
@@ -1440,7 +848,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1485,6 +892,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="457692432"/>
@@ -1526,6 +934,7 @@
       <a:pPr>
         <a:defRPr lang="en-US"/>
       </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1537,7 +946,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -1554,7 +963,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="marker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1584,9 +993,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
@@ -1619,8 +1025,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0667104111986002"/>
-                  <c:y val="0.300925925925926"/>
+                  <c:x val="-6.6710411198600203E-2"/>
+                  <c:y val="0.30092592592592599"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="#,##0.00_);[Red]\(#,##0.00\)" sourceLinked="0"/>
@@ -1648,6 +1054,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
+                  <a:endParaRPr lang="zh-CN"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1743,6 +1150,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DE64-4DB8-8445-F504DF7ECB4E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1789,7 +1201,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1834,6 +1245,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="457693088"/>
@@ -1874,7 +1286,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1919,6 +1330,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="457692432"/>
@@ -1960,6 +1372,7 @@
       <a:pPr>
         <a:defRPr lang="en-US"/>
       </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1971,7 +1384,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -1989,7 +1402,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="marker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -2019,9 +1432,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
@@ -2040,8 +1450,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.063255249343832"/>
-                  <c:y val="-0.0382531350247886"/>
+                  <c:x val="-6.3255249343832004E-2"/>
+                  <c:y val="-3.8253135024788602E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="#,##0.000000_);[Red]\(#,##0.000000\)" sourceLinked="0"/>
@@ -2069,6 +1479,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
+                  <a:endParaRPr lang="zh-CN"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2164,6 +1575,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D5EF-4026-A52F-2735D22F445F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2210,7 +1626,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2255,6 +1670,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="457693088"/>
@@ -2295,7 +1711,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2340,6 +1755,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="457692432"/>
@@ -2381,6 +1797,7 @@
       <a:pPr>
         <a:defRPr lang="en-US"/>
       </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2392,7 +1809,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -2410,7 +1827,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="marker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -2440,9 +1857,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
@@ -2461,8 +1875,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.063255249343832"/>
-                  <c:y val="-0.0382531350247886"/>
+                  <c:x val="-6.3255249343832004E-2"/>
+                  <c:y val="-3.8253135024788602E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="#,##0.000000_);[Red]\(#,##0.000000\)" sourceLinked="0"/>
@@ -2490,6 +1904,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
+                  <a:endParaRPr lang="zh-CN"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2585,6 +2000,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B18B-43FB-BEC1-B6F8C8A1CB1B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2631,7 +2051,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2676,6 +2095,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="457693088"/>
@@ -2716,7 +2136,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2761,6 +2180,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="457692432"/>
@@ -2802,6 +2222,7 @@
       <a:pPr>
         <a:defRPr lang="en-US"/>
       </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2814,7 +2235,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -2828,7 +2249,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2854,6 +2274,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2901,9 +2322,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>'ml0601'!$A$7:$A$87</c:f>
@@ -3166,22 +2584,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49.21342</c:v>
+                  <c:v>49.213419999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>134.93472</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>254.34702</c:v>
+                  <c:v>254.34701999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>404.71552</c:v>
+                  <c:v>404.71551999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>583.3875</c:v>
+                  <c:v>583.38750000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>787.79232</c:v>
+                  <c:v>787.7923199999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1015.44142</c:v>
@@ -3190,225 +2608,230 @@
                   <c:v>1263.92832</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1530.92862</c:v>
+                  <c:v>1530.9286200000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1814.2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2111.58222</c:v>
+                  <c:v>2111.5822199999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2420.99712</c:v>
+                  <c:v>2420.9971199999995</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2740.44862</c:v>
+                  <c:v>2740.4486199999997</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3068.02272</c:v>
+                  <c:v>3068.0227199999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3401.8875</c:v>
+                  <c:v>3401.8874999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3740.29312</c:v>
+                  <c:v>3740.2931199999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4081.57182</c:v>
+                  <c:v>4081.5718200000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4424.13792</c:v>
+                  <c:v>4424.1379200000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4766.48782</c:v>
+                  <c:v>4766.4878200000003</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>5107.2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5444.93502</c:v>
+                  <c:v>5444.935019999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>5778.43552</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6106.52622</c:v>
+                  <c:v>6106.5262199999997</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>6428.11392</c:v>
+                  <c:v>6428.1139199999989</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>6742.1875</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7047.81792</c:v>
+                  <c:v>7047.8179199999995</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7344.15822</c:v>
+                  <c:v>7344.1582199999993</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7630.44352</c:v>
+                  <c:v>7630.4435200000007</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7905.99102</c:v>
+                  <c:v>7905.9910199999995</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>8170.2</c:v>
+                  <c:v>8170.2000000000007</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8422.55182</c:v>
+                  <c:v>8422.5518200000006</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8662.60992</c:v>
+                  <c:v>8662.609919999999</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8890.01982</c:v>
+                  <c:v>8890.0198199999977</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>9104.50912</c:v>
+                  <c:v>9104.5091200000024</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>9305.8875</c:v>
+                  <c:v>9305.8875000000007</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>9494.04672</c:v>
+                  <c:v>9494.0467200000021</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>9668.96062</c:v>
+                  <c:v>9668.960619999998</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>9830.68512</c:v>
+                  <c:v>9830.6851199999983</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>9979.35822</c:v>
+                  <c:v>9979.3582200000019</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>10115.2</c:v>
+                  <c:v>10115.199999999997</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>10238.51262</c:v>
+                  <c:v>10238.512619999994</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>10349.68032</c:v>
+                  <c:v>10349.680319999992</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>10449.16942</c:v>
+                  <c:v>10449.169419999995</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>10537.52832</c:v>
+                  <c:v>10537.528320000001</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>10615.3875</c:v>
+                  <c:v>10615.387499999997</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>10683.45952</c:v>
+                  <c:v>10683.459519999997</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>10742.53902</c:v>
+                  <c:v>10742.539019999997</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>10793.50272</c:v>
+                  <c:v>10793.502719999997</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>10837.30942</c:v>
+                  <c:v>10837.30941999999</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>10875</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>10907.69742</c:v>
+                  <c:v>10907.697419999997</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>10936.60672</c:v>
+                  <c:v>10936.606719999996</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>10963.01502</c:v>
+                  <c:v>10963.015019999999</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>10988.29152</c:v>
+                  <c:v>10988.291519999999</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>11013.8875</c:v>
+                  <c:v>11013.887499999997</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>11041.33632</c:v>
+                  <c:v>11041.336320000002</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>11072.25342</c:v>
+                  <c:v>11072.253420000001</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>11108.33632</c:v>
+                  <c:v>11108.336319999995</c:v>
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>11151.36462</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>11203.2</c:v>
+                  <c:v>11203.199999999997</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>11265.78622</c:v>
+                  <c:v>11265.786219999995</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>11341.14912</c:v>
+                  <c:v>11341.149120000002</c:v>
                 </c:pt>
                 <c:pt idx="63">
                   <c:v>11431.39662</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>11538.71872</c:v>
+                  <c:v>11538.71871999999</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>11665.3875</c:v>
+                  <c:v>11665.387499999997</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>11813.75712</c:v>
+                  <c:v>11813.75711999998</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>11986.26382</c:v>
+                  <c:v>11986.263820000007</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>12185.42592</c:v>
+                  <c:v>12185.425920000009</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>12413.84382</c:v>
+                  <c:v>12413.843819999995</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>12674.2</c:v>
+                  <c:v>12674.199999999997</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>12969.25902</c:v>
+                  <c:v>12969.259020000012</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>13301.86752</c:v>
+                  <c:v>13301.867520000014</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>13674.95422</c:v>
+                  <c:v>13674.954220000014</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>14091.52992</c:v>
+                  <c:v>14091.529919999986</c:v>
                 </c:pt>
                 <c:pt idx="75">
                   <c:v>14554.6875</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>15067.60192</c:v>
+                  <c:v>15067.601920000001</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>15633.53022</c:v>
+                  <c:v>15633.530220000015</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>16255.81152</c:v>
+                  <c:v>16255.811520000017</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>16937.86702</c:v>
+                  <c:v>16937.86702000002</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>17683.2</c:v>
+                  <c:v>17683.199999999983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8503-4EB9-B2F7-BC4268171A61}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3476,6 +2899,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="431948607"/>
@@ -3537,6 +2961,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="400310924"/>
@@ -3577,6 +3002,7 @@
       <a:pPr>
         <a:defRPr lang="en-US"/>
       </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3584,7 +3010,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
-  <c:userShapes r:id="rId1"/>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -4145,7 +3571,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
@@ -4159,14 +3585,20 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="图表 2"/>
+        <xdr:cNvPr id="3" name="图表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4695825" y="1714500"/>
-        <a:ext cx="4572000" cy="2886075"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4189,14 +3621,20 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="图表 3"/>
+        <xdr:cNvPr id="4" name="图表 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9925050" y="1714500"/>
-        <a:ext cx="4572000" cy="2886075"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4210,7 +3648,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -4224,14 +3662,20 @@
       <xdr:row>22</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="图表 1"/>
+        <xdr:cNvPr id="2" name="图表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2066925" y="1343025"/>
-        <a:ext cx="4572000" cy="2886075"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4254,14 +3698,20 @@
       <xdr:row>41</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="图表 3"/>
+        <xdr:cNvPr id="4" name="图表 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2057400" y="4561840"/>
-        <a:ext cx="4572000" cy="3382010"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4284,14 +3734,20 @@
       <xdr:row>38</xdr:row>
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="图表 4"/>
+        <xdr:cNvPr id="5" name="图表 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7562215" y="2418715"/>
-        <a:ext cx="6124575" cy="4848225"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4315,12 +3771,12 @@
       <cdr:x>0.66407</cdr:x>
       <cdr:y>0.73292</cdr:y>
     </cdr:to>
-    <cdr:sp>
+    <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
         <cdr:cNvPr id="2" name="Straight Connector 1"/>
         <cdr:cNvSpPr/>
       </cdr:nvSpPr>
-      <cdr:spPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
           <a:off x="2838451" y="2476501"/>
           <a:ext cx="1228725" cy="895350"/>
@@ -4328,7 +3784,7 @@
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln w="22225">
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="22225">
           <a:solidFill>
             <a:srgbClr val="FF0000"/>
           </a:solidFill>
@@ -4354,7 +3810,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -4368,14 +3824,20 @@
       <xdr:row>38</xdr:row>
       <xdr:rowOff>164465</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3295650" y="1641475"/>
-        <a:ext cx="11191240" cy="5761990"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4398,9 +3860,15 @@
       <xdr:row>37</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp>
+    <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="2" name="Straight Connector 1"/>
+        <xdr:cNvPr id="2" name="Straight Connector 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -4442,9 +3910,15 @@
       <xdr:row>37</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp>
+    <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Connector 2"/>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -4473,6 +3947,1245 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="355675" cy="264560"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="文本框 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F2D2137-1CAD-4115-A4D8-1ED964400C02}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="12065000" y="6578600"/>
+              <a:ext cx="355675" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>0</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="文本框 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F2D2137-1CAD-4115-A4D8-1ED964400C02}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="12065000" y="6578600"/>
+              <a:ext cx="355675" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥_0</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="352404" cy="264560"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="文本框 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F346EFAA-41F1-4FCB-8862-884EF692FB7D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7118350" y="6731000"/>
+              <a:ext cx="352404" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="文本框 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F346EFAA-41F1-4FCB-8862-884EF692FB7D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7118350" y="6731000"/>
+              <a:ext cx="352404" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥_1</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="355675" cy="264560"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="文本框 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED7CDE1B-5D00-4098-8782-E1C737BD3212}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3657600" y="6711950"/>
+              <a:ext cx="355675" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="文本框 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED7CDE1B-5D00-4098-8782-E1C737BD3212}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3657600" y="6711950"/>
+              <a:ext cx="355675" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥_2</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="551177" cy="264560"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="文本框 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B780BC3-4346-4775-8C72-4E1D3BC40C8A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7239000" y="4654550"/>
+              <a:ext cx="551177" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>(</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>)</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="文本框 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B780BC3-4346-4775-8C72-4E1D3BC40C8A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7239000" y="4654550"/>
+              <a:ext cx="551177" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓(𝑥〗_1)</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="554446" cy="264560"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="文本框 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA353FF6-1690-48E3-A9D4-B3AF436990C4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="12217400" y="3435350"/>
+              <a:ext cx="554446" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>(</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>0</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>)</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="文本框 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA353FF6-1690-48E3-A9D4-B3AF436990C4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="12217400" y="3435350"/>
+              <a:ext cx="554446" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓(𝑥〗_0)</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>462644</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="759823" cy="264560"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="11" name="文本框 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1D7A8B7-208F-4727-A6E4-577C6297F567}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="12872358" y="2984500"/>
+              <a:ext cx="759823" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑦</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑓</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>(</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑥</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>)</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="11" name="文本框 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1D7A8B7-208F-4727-A6E4-577C6297F567}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="12872358" y="2984500"/>
+              <a:ext cx="759823" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑦</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>=𝑓(𝑥)</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>27214</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>72571</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="362728" cy="264560"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="文本框 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1219BD19-813D-40A3-BF57-D91060D88804}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9679214" y="6785428"/>
+              <a:ext cx="362728" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <m:rPr>
+                            <m:sty m:val="p"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>Δ</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="文本框 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1219BD19-813D-40A3-BF57-D91060D88804}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9679214" y="6785428"/>
+              <a:ext cx="362728" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>Δ_1</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>497114</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>16329</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="365998" cy="264560"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="13" name="文本框 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AEBF77E-AAD9-47C2-BFF5-7872267CA933}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5323114" y="6729186"/>
+              <a:ext cx="365998" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <m:rPr>
+                            <m:sty m:val="p"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>Δ</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="13" name="文本框 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AEBF77E-AAD9-47C2-BFF5-7872267CA933}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5323114" y="6729186"/>
+              <a:ext cx="365998" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>Δ_2</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4480,19 +5193,25 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.35661597821153</cdr:x>
-      <cdr:y>0.594555873925501</cdr:y>
+      <cdr:x>0.35662</cdr:x>
+      <cdr:y>0.59456</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.35661597821153</cdr:x>
-      <cdr:y>0.946660789067666</cdr:y>
+      <cdr:x>0.35662</cdr:x>
+      <cdr:y>0.94666</cdr:y>
     </cdr:to>
-    <cdr:cxnSp>
+    <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="2" name="Straight Connector 1"/>
+        <cdr:cNvPr id="2" name="Straight Connector 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE292893-7F0F-449A-8049-F8F0E8AD8CB6}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
         <cdr:cNvCxnSpPr/>
       </cdr:nvCxnSpPr>
-      <cdr:spPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="3990975" y="3425825"/>
           <a:ext cx="0" cy="2028825"/>
@@ -4519,19 +5238,25 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.0468111665910123</cdr:x>
-      <cdr:y>0.592902799206524</cdr:y>
+      <cdr:x>0.04681</cdr:x>
+      <cdr:y>0.5929</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.35661597821153</cdr:x>
-      <cdr:y>0.945007714348689</cdr:y>
+      <cdr:x>0.35662</cdr:x>
+      <cdr:y>0.94501</cdr:y>
     </cdr:to>
-    <cdr:cxnSp>
+    <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="3" name="Straight Connector 2"/>
+        <cdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0340322F-D4D1-48EE-A4F1-2ECD61F3A93D}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
         <cdr:cNvCxnSpPr/>
       </cdr:nvCxnSpPr>
-      <cdr:spPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
           <a:off x="523875" y="3416300"/>
           <a:ext cx="3467100" cy="2028825"/>
@@ -4811,6 +5536,7 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -5319,17 +6045,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5343,7 +6068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>20</v>
       </c>
@@ -5357,7 +6082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>40</v>
       </c>
@@ -5371,7 +6096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>60</v>
       </c>
@@ -5385,7 +6110,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>120</v>
       </c>
@@ -5399,7 +6124,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>160</v>
       </c>
@@ -5413,7 +6138,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>162</v>
       </c>
@@ -5427,12 +6152,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>171</v>
       </c>
       <c r="B8">
-        <v>17.1</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="D8">
         <v>171</v>
@@ -5442,25 +6167,24 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5468,7 +6192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -5476,7 +6200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10</v>
       </c>
@@ -5484,7 +6208,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>20</v>
       </c>
@@ -5492,7 +6216,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>40</v>
       </c>
@@ -5500,7 +6224,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>60</v>
       </c>
@@ -5508,7 +6232,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>80</v>
       </c>
@@ -5516,7 +6240,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>100</v>
       </c>
@@ -5524,7 +6248,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>120</v>
       </c>
@@ -5532,7 +6256,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>140</v>
       </c>
@@ -5540,7 +6264,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>160</v>
       </c>
@@ -5548,7 +6272,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>170</v>
       </c>
@@ -5556,7 +6280,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>180</v>
       </c>
@@ -5565,28 +6289,27 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5594,7 +6317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -5602,7 +6325,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -5610,7 +6333,7 @@
         <v>19.7</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -5618,15 +6341,15 @@
         <v>-0.49</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>0.00342</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>3.4199999999999999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -5634,817 +6357,818 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>0</v>
       </c>
       <c r="B7" s="1">
-        <f>$B$5*A7^4+$B$4*A7^3+$B$3*A7^2+$B$2*A7+$B$1</f>
+        <f t="shared" ref="B7:B38" si="0">$B$5*A7^4+$B$4*A7^3+$B$3*A7^2+$B$2*A7+$B$1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
       <c r="B8" s="1">
-        <f>$B$5*A8^4+$B$4*A8^3+$B$3*A8^2+$B$2*A8+$B$1</f>
-        <v>49.21342</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <f t="shared" si="0"/>
+        <v>49.213419999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <f t="shared" ref="A9:A72" si="0">A8+1</f>
+        <f t="shared" ref="A9:A72" si="1">A8+1</f>
         <v>2</v>
       </c>
       <c r="B9" s="1">
-        <f>$B$5*A9^4+$B$4*A9^3+$B$3*A9^2+$B$2*A9+$B$1</f>
+        <f t="shared" si="0"/>
         <v>134.93472</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B10" s="1">
-        <f>$B$5*A10^4+$B$4*A10^3+$B$3*A10^2+$B$2*A10+$B$1</f>
-        <v>254.34702</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>254.34701999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B11" s="1">
-        <f>$B$5*A11^4+$B$4*A11^3+$B$3*A11^2+$B$2*A11+$B$1</f>
-        <v>404.71552</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>404.71551999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B12" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B12" s="1">
-        <f>$B$5*A12^4+$B$4*A12^3+$B$3*A12^2+$B$2*A12+$B$1</f>
-        <v>583.3875</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>583.38750000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B13" s="1">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B13" s="1">
-        <f>$B$5*A13^4+$B$4*A13^3+$B$3*A13^2+$B$2*A13+$B$1</f>
-        <v>787.79232</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>787.7923199999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B14" s="1">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B14" s="1">
-        <f>$B$5*A14^4+$B$4*A14^3+$B$3*A14^2+$B$2*A14+$B$1</f>
         <v>1015.44142</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B15" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B15" s="1">
-        <f>$B$5*A15^4+$B$4*A15^3+$B$3*A15^2+$B$2*A15+$B$1</f>
         <v>1263.92832</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B16" s="1">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B16" s="1">
-        <f>$B$5*A16^4+$B$4*A16^3+$B$3*A16^2+$B$2*A16+$B$1</f>
-        <v>1530.92862</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>1530.9286200000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B17" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B17" s="1">
-        <f>$B$5*A17^4+$B$4*A17^3+$B$3*A17^2+$B$2*A17+$B$1</f>
         <v>1814.2</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B18" s="1">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B18" s="1">
-        <f>$B$5*A18^4+$B$4*A18^3+$B$3*A18^2+$B$2*A18+$B$1</f>
-        <v>2111.58222</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>2111.5822199999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B19" s="1">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B19" s="1">
-        <f>$B$5*A19^4+$B$4*A19^3+$B$3*A19^2+$B$2*A19+$B$1</f>
-        <v>2420.99712</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>2420.9971199999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B20" s="1">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B20" s="1">
-        <f>$B$5*A20^4+$B$4*A20^3+$B$3*A20^2+$B$2*A20+$B$1</f>
-        <v>2740.44862</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>2740.4486199999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B21" s="1">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B21" s="1">
-        <f>$B$5*A21^4+$B$4*A21^3+$B$3*A21^2+$B$2*A21+$B$1</f>
-        <v>3068.02272</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>3068.0227199999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B22" s="1">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B22" s="1">
-        <f>$B$5*A22^4+$B$4*A22^3+$B$3*A22^2+$B$2*A22+$B$1</f>
-        <v>3401.8875</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>3401.8874999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B23" s="1">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B23" s="1">
-        <f>$B$5*A23^4+$B$4*A23^3+$B$3*A23^2+$B$2*A23+$B$1</f>
-        <v>3740.29312</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>3740.2931199999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B24" s="1">
         <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B24" s="1">
-        <f>$B$5*A24^4+$B$4*A24^3+$B$3*A24^2+$B$2*A24+$B$1</f>
-        <v>4081.57182</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>4081.5718200000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B25" s="1">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B25" s="1">
-        <f>$B$5*A25^4+$B$4*A25^3+$B$3*A25^2+$B$2*A25+$B$1</f>
-        <v>4424.13792</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>4424.1379200000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B26" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B26" s="1">
-        <f>$B$5*A26^4+$B$4*A26^3+$B$3*A26^2+$B$2*A26+$B$1</f>
-        <v>4766.48782</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>4766.4878200000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B27" s="1">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B27" s="1">
-        <f>$B$5*A27^4+$B$4*A27^3+$B$3*A27^2+$B$2*A27+$B$1</f>
         <v>5107.2</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B28" s="1">
         <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B28" s="1">
-        <f>$B$5*A28^4+$B$4*A28^3+$B$3*A28^2+$B$2*A28+$B$1</f>
-        <v>5444.93502</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>5444.935019999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B29" s="1">
         <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B29" s="1">
-        <f>$B$5*A29^4+$B$4*A29^3+$B$3*A29^2+$B$2*A29+$B$1</f>
         <v>5778.43552</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B30" s="1">
         <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B30" s="1">
-        <f>$B$5*A30^4+$B$4*A30^3+$B$3*A30^2+$B$2*A30+$B$1</f>
-        <v>6106.52622</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>6106.5262199999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B31" s="1">
         <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B31" s="1">
-        <f>$B$5*A31^4+$B$4*A31^3+$B$3*A31^2+$B$2*A31+$B$1</f>
-        <v>6428.11392</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>6428.1139199999989</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B32" s="1">
         <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B32" s="1">
-        <f>$B$5*A32^4+$B$4*A32^3+$B$3*A32^2+$B$2*A32+$B$1</f>
         <v>6742.1875</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B33" s="1">
         <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B33" s="1">
-        <f>$B$5*A33^4+$B$4*A33^3+$B$3*A33^2+$B$2*A33+$B$1</f>
-        <v>7047.81792</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>7047.8179199999995</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B34" s="1">
         <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B34" s="1">
-        <f>$B$5*A34^4+$B$4*A34^3+$B$3*A34^2+$B$2*A34+$B$1</f>
-        <v>7344.15822</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>7344.1582199999993</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B35" s="1">
         <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B35" s="1">
-        <f>$B$5*A35^4+$B$4*A35^3+$B$3*A35^2+$B$2*A35+$B$1</f>
-        <v>7630.44352</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>7630.4435200000007</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B36" s="1">
         <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B36" s="1">
-        <f>$B$5*A36^4+$B$4*A36^3+$B$3*A36^2+$B$2*A36+$B$1</f>
-        <v>7905.99102</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>7905.9910199999995</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B37" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B37" s="1">
-        <f>$B$5*A37^4+$B$4*A37^3+$B$3*A37^2+$B$2*A37+$B$1</f>
-        <v>8170.2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>8170.2000000000007</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B38" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B38" s="1">
-        <f>$B$5*A38^4+$B$4*A38^3+$B$3*A38^2+$B$2*A38+$B$1</f>
-        <v>8422.55182</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>8422.5518200000006</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="B39" s="1">
-        <f>$B$5*A39^4+$B$4*A39^3+$B$3*A39^2+$B$2*A39+$B$1</f>
-        <v>8662.60992</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+        <f t="shared" ref="B39:B70" si="2">$B$5*A39^4+$B$4*A39^3+$B$3*A39^2+$B$2*A39+$B$1</f>
+        <v>8662.609919999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="B40" s="1">
-        <f>$B$5*A40^4+$B$4*A40^3+$B$3*A40^2+$B$2*A40+$B$1</f>
-        <v>8890.01982</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>8890.0198199999977</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B41" s="1">
-        <f>$B$5*A41^4+$B$4*A41^3+$B$3*A41^2+$B$2*A41+$B$1</f>
-        <v>9104.50912</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>9104.5091200000024</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B42" s="1">
-        <f>$B$5*A42^4+$B$4*A42^3+$B$3*A42^2+$B$2*A42+$B$1</f>
-        <v>9305.8875</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>9305.8875000000007</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B43" s="1">
-        <f>$B$5*A43^4+$B$4*A43^3+$B$3*A43^2+$B$2*A43+$B$1</f>
-        <v>9494.04672</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>9494.0467200000021</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B44" s="1">
-        <f>$B$5*A44^4+$B$4*A44^3+$B$3*A44^2+$B$2*A44+$B$1</f>
-        <v>9668.96062</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>9668.960619999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B45" s="1">
-        <f>$B$5*A45^4+$B$4*A45^3+$B$3*A45^2+$B$2*A45+$B$1</f>
-        <v>9830.68512</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>9830.6851199999983</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B46" s="1">
-        <f>$B$5*A46^4+$B$4*A46^3+$B$3*A46^2+$B$2*A46+$B$1</f>
-        <v>9979.35822</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>9979.3582200000019</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B47" s="1">
-        <f>$B$5*A47^4+$B$4*A47^3+$B$3*A47^2+$B$2*A47+$B$1</f>
-        <v>10115.2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>10115.199999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B48" s="1">
-        <f>$B$5*A48^4+$B$4*A48^3+$B$3*A48^2+$B$2*A48+$B$1</f>
-        <v>10238.51262</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>10238.512619999994</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B49" s="1">
-        <f>$B$5*A49^4+$B$4*A49^3+$B$3*A49^2+$B$2*A49+$B$1</f>
-        <v>10349.68032</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>10349.680319999992</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B50" s="1">
-        <f>$B$5*A50^4+$B$4*A50^3+$B$3*A50^2+$B$2*A50+$B$1</f>
-        <v>10449.16942</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>10449.169419999995</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="B51" s="1">
-        <f>$B$5*A51^4+$B$4*A51^3+$B$3*A51^2+$B$2*A51+$B$1</f>
-        <v>10537.52832</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>10537.528320000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="B52" s="1">
-        <f>$B$5*A52^4+$B$4*A52^3+$B$3*A52^2+$B$2*A52+$B$1</f>
-        <v>10615.3875</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>10615.387499999997</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="B53" s="1">
-        <f>$B$5*A53^4+$B$4*A53^3+$B$3*A53^2+$B$2*A53+$B$1</f>
-        <v>10683.45952</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>10683.459519999997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="B54" s="1">
-        <f>$B$5*A54^4+$B$4*A54^3+$B$3*A54^2+$B$2*A54+$B$1</f>
-        <v>10742.53902</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>10742.539019999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="B55" s="1">
-        <f>$B$5*A55^4+$B$4*A55^3+$B$3*A55^2+$B$2*A55+$B$1</f>
-        <v>10793.50272</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>10793.502719999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="B56" s="1">
-        <f>$B$5*A56^4+$B$4*A56^3+$B$3*A56^2+$B$2*A56+$B$1</f>
-        <v>10837.30942</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>10837.30941999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B57" s="1">
-        <f>$B$5*A57^4+$B$4*A57^3+$B$3*A57^2+$B$2*A57+$B$1</f>
+        <f t="shared" si="2"/>
         <v>10875</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="B58" s="1">
-        <f>$B$5*A58^4+$B$4*A58^3+$B$3*A58^2+$B$2*A58+$B$1</f>
-        <v>10907.69742</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>10907.697419999997</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="B59" s="1">
-        <f>$B$5*A59^4+$B$4*A59^3+$B$3*A59^2+$B$2*A59+$B$1</f>
-        <v>10936.60672</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>10936.606719999996</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="B60" s="1">
-        <f>$B$5*A60^4+$B$4*A60^3+$B$3*A60^2+$B$2*A60+$B$1</f>
-        <v>10963.01502</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>10963.015019999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="B61" s="1">
-        <f>$B$5*A61^4+$B$4*A61^3+$B$3*A61^2+$B$2*A61+$B$1</f>
-        <v>10988.29152</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>10988.291519999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="B62" s="1">
-        <f>$B$5*A62^4+$B$4*A62^3+$B$3*A62^2+$B$2*A62+$B$1</f>
-        <v>11013.8875</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>11013.887499999997</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="B63" s="1">
-        <f>$B$5*A63^4+$B$4*A63^3+$B$3*A63^2+$B$2*A63+$B$1</f>
-        <v>11041.33632</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>11041.336320000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="B64" s="1">
-        <f>$B$5*A64^4+$B$4*A64^3+$B$3*A64^2+$B$2*A64+$B$1</f>
-        <v>11072.25342</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>11072.253420000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="B65" s="1">
-        <f>$B$5*A65^4+$B$4*A65^3+$B$3*A65^2+$B$2*A65+$B$1</f>
-        <v>11108.33632</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>11108.336319999995</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="B66" s="1">
-        <f>$B$5*A66^4+$B$4*A66^3+$B$3*A66^2+$B$2*A66+$B$1</f>
+        <f t="shared" si="2"/>
         <v>11151.36462</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="B67" s="1">
-        <f>$B$5*A67^4+$B$4*A67^3+$B$3*A67^2+$B$2*A67+$B$1</f>
-        <v>11203.2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>11203.199999999997</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="B68" s="1">
-        <f>$B$5*A68^4+$B$4*A68^3+$B$3*A68^2+$B$2*A68+$B$1</f>
-        <v>11265.78622</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>11265.786219999995</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
       <c r="B69" s="1">
-        <f>$B$5*A69^4+$B$4*A69^3+$B$3*A69^2+$B$2*A69+$B$1</f>
-        <v>11341.14912</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
+        <f t="shared" si="2"/>
+        <v>11341.149120000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="B70" s="1">
-        <f>$B$5*A70^4+$B$4*A70^3+$B$3*A70^2+$B$2*A70+$B$1</f>
+        <f t="shared" si="2"/>
         <v>11431.39662</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="B71" s="1">
-        <f>$B$5*A71^4+$B$4*A71^3+$B$3*A71^2+$B$2*A71+$B$1</f>
-        <v>11538.71872</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
+        <f t="shared" ref="B71:B102" si="3">$B$5*A71^4+$B$4*A71^3+$B$3*A71^2+$B$2*A71+$B$1</f>
+        <v>11538.71871999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
       <c r="B72" s="1">
-        <f>$B$5*A72^4+$B$4*A72^3+$B$3*A72^2+$B$2*A72+$B$1</f>
-        <v>11665.3875</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
+        <f t="shared" si="3"/>
+        <v>11665.387499999997</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
-        <f t="shared" ref="A73:A87" si="1">A72+1</f>
+        <f t="shared" ref="A73:A87" si="4">A72+1</f>
         <v>66</v>
       </c>
       <c r="B73" s="1">
-        <f>$B$5*A73^4+$B$4*A73^3+$B$3*A73^2+$B$2*A73+$B$1</f>
-        <v>11813.75712</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
+        <f t="shared" si="3"/>
+        <v>11813.75711999998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>67</v>
       </c>
       <c r="B74" s="1">
-        <f>$B$5*A74^4+$B$4*A74^3+$B$3*A74^2+$B$2*A74+$B$1</f>
-        <v>11986.26382</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
+        <f t="shared" si="3"/>
+        <v>11986.263820000007</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>68</v>
       </c>
       <c r="B75" s="1">
-        <f>$B$5*A75^4+$B$4*A75^3+$B$3*A75^2+$B$2*A75+$B$1</f>
-        <v>12185.42592</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
+        <f t="shared" si="3"/>
+        <v>12185.425920000009</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>69</v>
       </c>
       <c r="B76" s="1">
-        <f>$B$5*A76^4+$B$4*A76^3+$B$3*A76^2+$B$2*A76+$B$1</f>
-        <v>12413.84382</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
+        <f t="shared" si="3"/>
+        <v>12413.843819999995</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="B77" s="1">
-        <f>$B$5*A77^4+$B$4*A77^3+$B$3*A77^2+$B$2*A77+$B$1</f>
-        <v>12674.2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
+        <f t="shared" si="3"/>
+        <v>12674.199999999997</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>71</v>
       </c>
       <c r="B78" s="1">
-        <f>$B$5*A78^4+$B$4*A78^3+$B$3*A78^2+$B$2*A78+$B$1</f>
-        <v>12969.25902</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
+        <f t="shared" si="3"/>
+        <v>12969.259020000012</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>72</v>
       </c>
       <c r="B79" s="1">
-        <f>$B$5*A79^4+$B$4*A79^3+$B$3*A79^2+$B$2*A79+$B$1</f>
-        <v>13301.86752</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
+        <f t="shared" si="3"/>
+        <v>13301.867520000014</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>73</v>
       </c>
       <c r="B80" s="1">
-        <f>$B$5*A80^4+$B$4*A80^3+$B$3*A80^2+$B$2*A80+$B$1</f>
-        <v>13674.95422</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
+        <f t="shared" si="3"/>
+        <v>13674.954220000014</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
       <c r="B81" s="1">
-        <f>$B$5*A81^4+$B$4*A81^3+$B$3*A81^2+$B$2*A81+$B$1</f>
-        <v>14091.52992</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
+        <f t="shared" si="3"/>
+        <v>14091.529919999986</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>75</v>
       </c>
       <c r="B82" s="1">
-        <f>$B$5*A82^4+$B$4*A82^3+$B$3*A82^2+$B$2*A82+$B$1</f>
+        <f t="shared" si="3"/>
         <v>14554.6875</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>76</v>
       </c>
       <c r="B83" s="1">
-        <f>$B$5*A83^4+$B$4*A83^3+$B$3*A83^2+$B$2*A83+$B$1</f>
-        <v>15067.60192</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
+        <f t="shared" si="3"/>
+        <v>15067.601920000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>77</v>
       </c>
       <c r="B84" s="1">
-        <f>$B$5*A84^4+$B$4*A84^3+$B$3*A84^2+$B$2*A84+$B$1</f>
-        <v>15633.53022</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
+        <f t="shared" si="3"/>
+        <v>15633.530220000015</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>78</v>
       </c>
       <c r="B85" s="1">
-        <f>$B$5*A85^4+$B$4*A85^3+$B$3*A85^2+$B$2*A85+$B$1</f>
-        <v>16255.81152</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
+        <f t="shared" si="3"/>
+        <v>16255.811520000017</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>79</v>
       </c>
       <c r="B86" s="1">
-        <f>$B$5*A86^4+$B$4*A86^3+$B$3*A86^2+$B$2*A86+$B$1</f>
-        <v>16937.86702</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
+        <f t="shared" si="3"/>
+        <v>16937.86702000002</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="B87" s="1">
-        <f>$B$5*A87^4+$B$4*A87^3+$B$3*A87^2+$B$2*A87+$B$1</f>
-        <v>17683.2</v>
+        <f t="shared" si="3"/>
+        <v>17683.199999999983</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>